<commit_message>
chore!: update input files.
Update documentation in input files.
XLENGTH -> ZLENGTH in template_conductor_definition.
</commit_message>
<xml_diff>
--- a/source_code/input_files/input_file_template/template_conductor_1_input.xlsx
+++ b/source_code/input_files/input_file_template/template_conductor_1_input.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/daniele_placido_polito_it/Documents/OPENSC2/source_code/Description_of_Components/input_file_template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/daniele_placido_polito_it/Documents/OPENSC2/source_code/input_files/input_file_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="167" documentId="13_ncr:1_{0BD40D79-8656-4BCB-943B-68FA050A86D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD15AF16-C13E-4A87-98F1-0989E9B0A80C}"/>
+  <xr:revisionPtr revIDLastSave="178" documentId="13_ncr:1_{0BD40D79-8656-4BCB-943B-68FA050A86D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5FBF9883-5653-4504-A127-1D67BFA12721}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="2250" windowWidth="21600" windowHeight="11385" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CHAN" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="96">
   <si>
     <t>COSTETA</t>
   </si>
@@ -318,13 +318,16 @@
     <t>X_barycenter</t>
   </si>
   <si>
-    <t>x coordinate of the barycenter</t>
-  </si>
-  <si>
     <t>Y_barycenter</t>
   </si>
   <si>
-    <t>y coordinate of the barycenter</t>
+    <t>x coordinate of the barycenter. Not used if flag ITYMESH = -1 in file conductor_grid.</t>
+  </si>
+  <si>
+    <t>y coordinate of the barycenter Not used if flag ITYMESH = -1 in file conductor_grid.</t>
+  </si>
+  <si>
+    <t>y coordinate of the barycenter. Not used if flag ITYMESH = -1 in file conductor_grid.</t>
   </si>
 </sst>
 </file>
@@ -850,20 +853,20 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E5" sqref="E5:F6"/>
+      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="68" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="17.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="3"/>
+    <col min="5" max="6" width="17.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.81640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>5</v>
       </c>
@@ -881,7 +884,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="D2" s="4" t="s">
@@ -896,7 +899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="str">
         <f>[1]TRANSIENT!A$2</f>
         <v>Variable name</v>
@@ -922,7 +925,7 @@
         <v>CHAN_2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -942,7 +945,7 @@
         <v>3.6965000000000001E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>91</v>
       </c>
@@ -953,18 +956,18 @@
         <v>18</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="23">
+        <v>0</v>
+      </c>
+      <c r="F5" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="E5" s="23">
-        <v>0</v>
-      </c>
-      <c r="F5" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>93</v>
       </c>
       <c r="B6" s="22" t="s">
         <v>9</v>
@@ -973,7 +976,7 @@
         <v>18</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E6" s="23">
         <v>0</v>
@@ -982,7 +985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
@@ -1002,7 +1005,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -1022,7 +1025,7 @@
         <v>3.2676E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>85</v>
       </c>
@@ -1042,7 +1045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>0</v>
       </c>
@@ -1062,7 +1065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
@@ -1082,7 +1085,7 @@
         <v>0.313</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
@@ -1102,7 +1105,7 @@
         <v>-99</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
         <v>11</v>
       </c>
@@ -1122,7 +1125,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
@@ -1141,7 +1144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
@@ -1158,7 +1161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
@@ -1175,7 +1178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>56</v>
       </c>
@@ -1195,7 +1198,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>62</v>
       </c>
@@ -1215,7 +1218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>87</v>
       </c>
@@ -1250,20 +1253,20 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5:XFD6"/>
+      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="67.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="67.1796875" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="3"/>
+    <col min="6" max="16384" width="8.81640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>1</v>
       </c>
@@ -1279,7 +1282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1291,7 +1294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="str">
         <f>CHAN!A3</f>
         <v>Variable name</v>
@@ -1313,7 +1316,7 @@
         <v>STR_MIX_1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -1331,7 +1334,7 @@
         <v>7.5395176499999997E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>91</v>
       </c>
@@ -1342,15 +1345,15 @@
         <v>18</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="E5" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>93</v>
       </c>
       <c r="B6" s="22" t="s">
         <v>9</v>
@@ -1359,13 +1362,13 @@
         <v>18</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E6" s="23">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
@@ -1382,7 +1385,7 @@
         <v>0.96989999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>34</v>
       </c>
@@ -1399,7 +1402,7 @@
         <v>2.0846</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>37</v>
       </c>
@@ -1416,7 +1419,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
@@ -1433,7 +1436,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
@@ -1450,7 +1453,7 @@
         <v>197.71</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
         <v>35</v>
       </c>
@@ -1467,7 +1470,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
         <v>77</v>
       </c>
@@ -1484,7 +1487,7 @@
         <v>121508000000</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
         <v>78</v>
       </c>
@@ -1501,7 +1504,7 @@
         <v>32.35</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
         <v>79</v>
       </c>
@@ -1518,7 +1521,7 @@
         <v>16.22</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>87</v>
       </c>
@@ -1550,20 +1553,20 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5:XFD6"/>
+      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="67.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="3"/>
+    <col min="2" max="2" width="7.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="67.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.81640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>15</v>
       </c>
@@ -1579,7 +1582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1591,7 +1594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="str">
         <f>CHAN!A3</f>
         <v>Variable name</v>
@@ -1613,7 +1616,7 @@
         <v>STR_SC_0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -1630,7 +1633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>91</v>
       </c>
@@ -1641,15 +1644,15 @@
         <v>18</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="E5" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>93</v>
       </c>
       <c r="B6" s="22" t="s">
         <v>9</v>
@@ -1658,13 +1661,13 @@
         <v>18</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E6" s="23">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
@@ -1681,7 +1684,7 @@
         <v>0.96989999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
         <v>35</v>
       </c>
@@ -1698,7 +1701,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
         <v>77</v>
       </c>
@@ -1715,7 +1718,7 @@
         <v>170360000000000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>78</v>
       </c>
@@ -1732,7 +1735,7 @@
         <v>30.23</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>79</v>
       </c>
@@ -1749,7 +1752,7 @@
         <v>16.73</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>87</v>
       </c>
@@ -1777,24 +1780,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDD13407-BFB1-4787-A354-6C7A2E5E5AE6}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5:XFD6"/>
+      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="3"/>
+    <col min="1" max="1" width="13.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.81640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>36</v>
       </c>
@@ -1810,7 +1813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1822,7 +1825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="str">
         <f>CHAN!A3</f>
         <v>Variable name</v>
@@ -1844,7 +1847,7 @@
         <v>STR_STAB_0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -1861,7 +1864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>91</v>
       </c>
@@ -1872,15 +1875,15 @@
         <v>18</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="E5" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>93</v>
       </c>
       <c r="B6" s="22" t="s">
         <v>9</v>
@@ -1889,13 +1892,13 @@
         <v>18</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E6" s="23">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
@@ -1912,7 +1915,7 @@
         <v>0.96989999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -1929,7 +1932,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1946,7 +1949,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>87</v>
       </c>
@@ -1974,24 +1977,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="3"/>
+    <col min="1" max="1" width="20.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.81640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>17</v>
       </c>
@@ -2007,7 +2010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2019,7 +2022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="str">
         <f>CHAN!A3</f>
         <v>Variable name</v>
@@ -2041,7 +2044,7 @@
         <v>Z_JACKET_1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -2059,7 +2062,7 @@
         <v>3.0698999999999999E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -2076,7 +2079,7 @@
         <v>2.7965999999999999E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>91</v>
       </c>
@@ -2087,15 +2090,15 @@
         <v>18</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E6" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="E6" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>93</v>
       </c>
       <c r="B7" s="22" t="s">
         <v>9</v>
@@ -2110,7 +2113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>81</v>
       </c>
@@ -2127,7 +2130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>83</v>
       </c>
@@ -2144,7 +2147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>37</v>
       </c>
@@ -2161,7 +2164,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="28" t="s">
         <v>32</v>
       </c>
@@ -2178,7 +2181,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>33</v>
       </c>
@@ -2195,7 +2198,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>0</v>
       </c>
@@ -2209,7 +2212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="28" t="s">
         <v>70</v>
       </c>
@@ -2226,7 +2229,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>72</v>
       </c>
@@ -2243,7 +2246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>87</v>
       </c>

</xml_diff>

<commit_message>
chore: rename input variable name in file template_conductor_1_input.xlsx.
Renamed:

* ISTABILIZER to stabilizer_material
* ISUPERCONDUCTOR to superconducting_material
* IMATERIAL_JK to jacket_material
* IMATERIAL_IN to insulation_material
* CROSSECTION_JK to jacket_cross_section
* CROSSECTION_IN to insulation_cross_section
* "None" to "none"
* HTS with YBCO (the only one available at the time being)
</commit_message>
<xml_diff>
--- a/source_code/input_files/input_file_template/template_conductor_1_input.xlsx
+++ b/source_code/input_files/input_file_template/template_conductor_1_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/daniele_placido_polito_it/Documents/OPENSC2/source_code/input_files/input_file_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="178" documentId="13_ncr:1_{0BD40D79-8656-4BCB-943B-68FA050A86D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5FBF9883-5653-4504-A127-1D67BFA12721}"/>
+  <xr:revisionPtr revIDLastSave="189" documentId="13_ncr:1_{0BD40D79-8656-4BCB-943B-68FA050A86D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B22F3491-E4CA-40BC-A85F-0A53FDA4F5CB}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CHAN" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="98">
   <si>
     <t>COSTETA</t>
   </si>
@@ -48,12 +48,6 @@
     <t>STR_MIX</t>
   </si>
   <si>
-    <t>CROSSECTION_JK</t>
-  </si>
-  <si>
-    <t>CROSSECTION_IN</t>
-  </si>
-  <si>
     <t>CROSSECTION</t>
   </si>
   <si>
@@ -90,9 +84,6 @@
     <t>STR_SC</t>
   </si>
   <si>
-    <t>ISTABILIZER</t>
-  </si>
-  <si>
     <t>Z_JACKET</t>
   </si>
   <si>
@@ -138,12 +129,6 @@
     <t>row used to get the correct number of jacket objects in cell B1 as the sum of values in this row starting from cell D2</t>
   </si>
   <si>
-    <t>IMATERIAL_JK</t>
-  </si>
-  <si>
-    <t>IMATERIAL_IN</t>
-  </si>
-  <si>
     <t>STAB_NON_STAB</t>
   </si>
   <si>
@@ -267,12 +252,6 @@
     <t>whole_enclosure</t>
   </si>
   <si>
-    <t>Flag, glass_epoxy = glass epoxy; None = pure metal component</t>
-  </si>
-  <si>
-    <t>Flag, steinless_steel = steinless steel (old Fortran IJK); None = insulation component</t>
-  </si>
-  <si>
     <t>c0</t>
   </si>
   <si>
@@ -328,6 +307,33 @@
   </si>
   <si>
     <t>y coordinate of the barycenter. Not used if flag ITYMESH = -1 in file conductor_grid.</t>
+  </si>
+  <si>
+    <t>stabilizer_material</t>
+  </si>
+  <si>
+    <t>superconducting_material</t>
+  </si>
+  <si>
+    <t>jacket_cross_section</t>
+  </si>
+  <si>
+    <t>insulation_cross_section</t>
+  </si>
+  <si>
+    <t>jacket_material</t>
+  </si>
+  <si>
+    <t>insulation_material</t>
+  </si>
+  <si>
+    <t>Flag, steinless_steel = steinless steel (old Fortran IJK); none = insulation component</t>
+  </si>
+  <si>
+    <t>Flag, glass_epoxy = glass epoxy; none = pure metal component</t>
+  </si>
+  <si>
+    <t>flag for material: NbTi = niobiun titanium, Nb3Sn = niobium thin, YBCO = YBCO (REBCO)</t>
   </si>
 </sst>
 </file>
@@ -868,14 +874,14 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B1" s="14">
         <f>SUM(E$2:U$2)</f>
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E1" s="2">
         <v>1</v>
@@ -888,7 +894,7 @@
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="D2" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E2" s="14">
         <f>IF(E$1 &gt; 0,1,0)</f>
@@ -927,16 +933,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E4" s="19">
         <v>5.0265000000000001E-5</v>
@@ -947,16 +953,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E5" s="23">
         <v>0</v>
@@ -967,16 +973,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E6" s="23">
         <v>0</v>
@@ -987,36 +993,36 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E8" s="20">
         <v>8.0000000000000002E-3</v>
@@ -1027,16 +1033,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E9" s="24">
         <v>0</v>
@@ -1050,13 +1056,13 @@
         <v>0</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E10" s="21">
         <v>1</v>
@@ -1067,16 +1073,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E11" s="18">
         <v>1</v>
@@ -1087,16 +1093,16 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E12" s="18">
         <v>-99</v>
@@ -1107,16 +1113,16 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E13" s="18">
         <v>0.02</v>
@@ -1127,13 +1133,13 @@
     </row>
     <row r="14" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E14" s="18" t="b">
         <f>FALSE</f>
@@ -1146,13 +1152,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E15" s="19">
         <v>0</v>
@@ -1163,13 +1169,13 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E16" s="19">
         <v>0</v>
@@ -1180,36 +1186,36 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E18" s="5">
         <v>1</v>
@@ -1220,16 +1226,16 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E19" s="22" t="b">
         <v>0</v>
@@ -1253,7 +1259,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1276,7 +1282,7 @@
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E1" s="11">
         <v>1</v>
@@ -1287,7 +1293,7 @@
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E2" s="15">
         <f>IF(E$1 &gt; 0,1,0)</f>
@@ -1318,16 +1324,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E4" s="23">
         <f>(0.00052534+0.00025201)*E7</f>
@@ -1336,16 +1342,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E5" s="23">
         <v>0</v>
@@ -1353,16 +1359,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E6" s="23">
         <v>0</v>
@@ -1373,13 +1379,13 @@
         <v>0</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E7" s="24">
         <v>0.96989999999999998</v>
@@ -1387,16 +1393,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E8" s="24">
         <v>2.0846</v>
@@ -1404,16 +1410,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E9" s="25">
         <v>2</v>
@@ -1421,33 +1427,33 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>19</v>
-      </c>
       <c r="D10" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E11" s="26">
         <v>197.71</v>
@@ -1455,33 +1461,33 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
-        <v>35</v>
+        <v>90</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>64</v>
+        <v>97</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E13" s="29">
         <v>121508000000</v>
@@ -1489,16 +1495,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E14" s="29">
         <v>32.35</v>
@@ -1506,16 +1512,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E15" s="29">
         <v>16.22</v>
@@ -1523,16 +1529,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E16" s="22" t="b">
         <v>0</v>
@@ -1568,7 +1574,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B1" s="14">
         <f>SUM(E$2:Z2)</f>
@@ -1576,7 +1582,7 @@
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E1" s="11">
         <v>0</v>
@@ -1587,7 +1593,7 @@
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E2" s="15">
         <f>IF(E$1 &gt; 0,1,0)</f>
@@ -1618,16 +1624,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E4" s="13">
         <v>0</v>
@@ -1635,16 +1641,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E5" s="23">
         <v>0</v>
@@ -1652,16 +1658,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E6" s="23">
         <v>0</v>
@@ -1672,13 +1678,13 @@
         <v>0</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E7" s="7">
         <v>0.96989999999999998</v>
@@ -1686,33 +1692,33 @@
     </row>
     <row r="8" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E9" s="29">
         <v>170360000000000</v>
@@ -1720,16 +1726,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E10" s="21">
         <v>30.23</v>
@@ -1737,16 +1743,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E11" s="21">
         <v>16.73</v>
@@ -1754,16 +1760,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E12" s="22" t="b">
         <v>1</v>
@@ -1780,11 +1786,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDD13407-BFB1-4787-A354-6C7A2E5E5AE6}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1799,7 +1805,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B1" s="14">
         <f>SUM(E$2:Z2)</f>
@@ -1807,7 +1813,7 @@
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E1" s="2">
         <v>0</v>
@@ -1818,7 +1824,7 @@
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="17" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E2" s="14">
         <f>IF(E$1 &gt; 0,1,0)</f>
@@ -1849,16 +1855,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E4" s="13">
         <v>0</v>
@@ -1866,16 +1872,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E5" s="23">
         <v>0</v>
@@ -1883,16 +1889,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E6" s="23">
         <v>0</v>
@@ -1903,13 +1909,13 @@
         <v>0</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E7" s="7">
         <v>0.96989999999999998</v>
@@ -1917,33 +1923,33 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>19</v>
-      </c>
       <c r="D8" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E9" s="12">
         <v>100</v>
@@ -1951,16 +1957,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E10" s="22" t="b">
         <v>1</v>
@@ -1977,11 +1983,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomRight" activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1996,7 +2002,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B1" s="14">
         <f>SUM(E$2:Z2)</f>
@@ -2004,7 +2010,7 @@
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E1" s="11">
         <v>1</v>
@@ -2015,7 +2021,7 @@
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E2" s="15">
         <f>IF(E$1 &gt; 0,1,0)</f>
@@ -2046,16 +2052,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>2</v>
+        <v>91</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E4" s="6">
         <f>0.00030699</f>
@@ -2064,16 +2070,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>3</v>
+        <v>92</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E5" s="6">
         <v>2.7965999999999999E-4</v>
@@ -2081,16 +2087,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E6" s="23">
         <v>0</v>
@@ -2098,16 +2104,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="E7" s="23">
         <v>0</v>
@@ -2115,16 +2121,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E8" s="23">
         <v>0</v>
@@ -2132,16 +2138,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E9" s="23">
         <v>0</v>
@@ -2149,16 +2155,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E10" s="12">
         <v>2</v>
@@ -2166,36 +2172,36 @@
     </row>
     <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="28" t="s">
-        <v>32</v>
+        <v>93</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>33</v>
+        <v>94</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -2203,10 +2209,10 @@
         <v>0</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E13" s="6">
         <v>1</v>
@@ -2214,33 +2220,33 @@
     </row>
     <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="28" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E14" s="27" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E15" s="22">
         <v>1</v>
@@ -2248,16 +2254,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="E16" s="22" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
feat!: new input files for StakComponent object.
Defined input files for the new object StakComponent.
</commit_message>
<xml_diff>
--- a/source_code/input_files/input_file_template/template_conductor_1_input.xlsx
+++ b/source_code/input_files/input_file_template/template_conductor_1_input.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/daniele_placido_polito_it/Documents/OPENSC2/source_code/input_files/input_file_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="189" documentId="13_ncr:1_{0BD40D79-8656-4BCB-943B-68FA050A86D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B22F3491-E4CA-40BC-A85F-0A53FDA4F5CB}"/>
+  <xr:revisionPtr revIDLastSave="280" documentId="13_ncr:1_{0BD40D79-8656-4BCB-943B-68FA050A86D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B79F21B8-56E2-4D4E-9ECB-A48BD02ED969}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CHAN" sheetId="2" r:id="rId1"/>
-    <sheet name="STR_MIX" sheetId="3" r:id="rId2"/>
-    <sheet name="STR_SC" sheetId="5" r:id="rId3"/>
+    <sheet name="STACK" sheetId="5" r:id="rId2"/>
+    <sheet name="STR_MIX" sheetId="3" r:id="rId3"/>
     <sheet name="STR_STAB" sheetId="6" r:id="rId4"/>
     <sheet name="Z_JACKET" sheetId="4" r:id="rId5"/>
   </sheets>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="128">
   <si>
     <t>COSTETA</t>
   </si>
@@ -81,9 +81,6 @@
     <t>SIDE2</t>
   </si>
   <si>
-    <t>STR_SC</t>
-  </si>
-  <si>
     <t>Z_JACKET</t>
   </si>
   <si>
@@ -132,9 +129,6 @@
     <t>STAB_NON_STAB</t>
   </si>
   <si>
-    <t>ISUPERCONDUCTOR</t>
-  </si>
-  <si>
     <t>STR_STAB</t>
   </si>
   <si>
@@ -219,9 +213,6 @@
     <t>flag to select the correlation used to evaluate the channel steady state heat transfer coefficient</t>
   </si>
   <si>
-    <t>flag for material: NbTi = niobiun titanium, Nb3Sn = niobium thin, HTS = high critical temperature superconducting material, scaling.dat = scaling from file scaling.dat</t>
-  </si>
-  <si>
     <t>Nb3Sn</t>
   </si>
   <si>
@@ -334,6 +325,105 @@
   </si>
   <si>
     <t>flag for material: NbTi = niobiun titanium, Nb3Sn = niobium thin, YBCO = YBCO (REBCO)</t>
+  </si>
+  <si>
+    <t>STACK</t>
+  </si>
+  <si>
+    <t>Tape_number</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>Number of tapes constituting the stack</t>
+  </si>
+  <si>
+    <t>Stack_witdh</t>
+  </si>
+  <si>
+    <t>Width of the stack of tapes</t>
+  </si>
+  <si>
+    <t>Stabilizer_thickness</t>
+  </si>
+  <si>
+    <t>Overlayer_thickness</t>
+  </si>
+  <si>
+    <t>HTS_thickness</t>
+  </si>
+  <si>
+    <t>Substrate_thickness</t>
+  </si>
+  <si>
+    <t>Solder_thickness</t>
+  </si>
+  <si>
+    <t>Stabilizer_material</t>
+  </si>
+  <si>
+    <t>Overlayer_material</t>
+  </si>
+  <si>
+    <t>HTS_material</t>
+  </si>
+  <si>
+    <t>Substrate_material</t>
+  </si>
+  <si>
+    <t>Solder_material</t>
+  </si>
+  <si>
+    <t>HTS material: YBCO = REBCO with RE = Yttrium; Bi2223 = 1G material (not available); Bi2212 = 1G material (not available);</t>
+  </si>
+  <si>
+    <t>Stabilizer material: cu = copper; al = alluminium; none = no stabilizer</t>
+  </si>
+  <si>
+    <t>Overlayer material: cu = copper; al = alluminium; none = no overlayer</t>
+  </si>
+  <si>
+    <t>Substrate material: hc276 = hastelloy 276; none = no substrate</t>
+  </si>
+  <si>
+    <t>Stabilizer material: Sn60Pb40 = solder alloy 60% tin 40% led ; none = no solder</t>
+  </si>
+  <si>
+    <t>nn</t>
+  </si>
+  <si>
+    <t>E0</t>
+  </si>
+  <si>
+    <t>V/m</t>
+  </si>
+  <si>
+    <t>Reference electric field for the power law, used to evaluate superconducting electrical resistivity. Defaults to 10^-5 V/m</t>
+  </si>
+  <si>
+    <t>Power low exponent assumed independent of the temperature, used to evaluate superconducting electrical resistivity. Default to 20.</t>
+  </si>
+  <si>
+    <t>Total thickness of the stabilizer layer; set to 0 if no stabilizer.</t>
+  </si>
+  <si>
+    <t>Total thickness of the overlayer layer; set to 0 if no overlayer.</t>
+  </si>
+  <si>
+    <t>Total thickness of the HTS layer.</t>
+  </si>
+  <si>
+    <t>Total thickness of the substrate layer; set to 0 if no substrate.</t>
+  </si>
+  <si>
+    <t>Total thickness of the solder layer; set to 0 if no solder.</t>
+  </si>
+  <si>
+    <t>Material_number</t>
+  </si>
+  <si>
+    <t>Number of materials constituting the tape.</t>
   </si>
 </sst>
 </file>
@@ -401,7 +491,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
@@ -509,6 +599,10 @@
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -881,7 +975,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E1" s="2">
         <v>1</v>
@@ -894,7 +988,7 @@
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="D2" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2" s="14">
         <f>IF(E$1 &gt; 0,1,0)</f>
@@ -939,10 +1033,10 @@
         <v>6</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E4" s="19">
         <v>5.0265000000000001E-5</v>
@@ -953,16 +1047,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B5" s="22" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E5" s="23">
         <v>0</v>
@@ -973,16 +1067,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B6" s="22" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E6" s="23">
         <v>0</v>
@@ -993,22 +1087,22 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
@@ -1019,10 +1113,10 @@
         <v>7</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E8" s="20">
         <v>8.0000000000000002E-3</v>
@@ -1033,16 +1127,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B9" s="22" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E9" s="24">
         <v>0</v>
@@ -1056,13 +1150,13 @@
         <v>0</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E10" s="21">
         <v>1</v>
@@ -1073,16 +1167,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E11" s="18">
         <v>1</v>
@@ -1096,13 +1190,13 @@
         <v>8</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E12" s="18">
         <v>-99</v>
@@ -1116,13 +1210,13 @@
         <v>9</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E13" s="18">
         <v>0.02</v>
@@ -1136,10 +1230,10 @@
         <v>10</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E14" s="18" t="b">
         <f>FALSE</f>
@@ -1158,7 +1252,7 @@
         <v>7</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E15" s="19">
         <v>0</v>
@@ -1175,7 +1269,7 @@
         <v>7</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E16" s="19">
         <v>0</v>
@@ -1186,36 +1280,36 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="3" t="s">
+      <c r="F17" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E18" s="5">
         <v>1</v>
@@ -1226,16 +1320,16 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E19" s="22" t="b">
         <v>0</v>
@@ -1252,6 +1346,452 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62FCDFC4-8F8B-44BE-BC94-0C08DE31F1F6}">
+  <dimension ref="A1:E26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="67.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.81640625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="14">
+        <f>SUM(E$2:Z2)</f>
+        <v>0</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="15">
+        <f>IF(E$1 &gt; 0,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="16" t="str">
+        <f>CHAN!A3</f>
+        <v>Variable name</v>
+      </c>
+      <c r="B3" s="16" t="str">
+        <f>CHAN!B3</f>
+        <v>Unit</v>
+      </c>
+      <c r="C3" s="16" t="str">
+        <f>CHAN!C3</f>
+        <v>Variable type</v>
+      </c>
+      <c r="D3" s="16" t="str">
+        <f>CHAN!D3</f>
+        <v>Note/comments</v>
+      </c>
+      <c r="E3" s="14" t="str">
+        <f>_xlfn.TEXTJOIN("_",,$A$1,E$1)</f>
+        <v>STACK_0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="E6" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="24">
+        <v>0.96989999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="E8" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="E9" s="24"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="E10" s="24"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="E11" s="24"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="E12" s="24"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="E13" s="24"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="E14" s="24"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="E15" s="24"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="E16" s="24"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="E17" s="24"/>
+    </row>
+    <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="E18" s="24"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="E19" s="24"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="E20" s="24"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" s="29">
+        <v>170360000000000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="E22" s="21">
+        <v>30.23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23" s="21">
+        <v>16.73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="D24" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="E24" s="21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="E25" s="21">
+        <f>10^-5</f>
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="E26" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
@@ -1282,310 +1822,10 @@
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E1" s="11">
         <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="15">
-        <f>IF(E$1 &gt; 0,1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="16" t="str">
-        <f>CHAN!A3</f>
-        <v>Variable name</v>
-      </c>
-      <c r="B3" s="16" t="str">
-        <f>CHAN!B3</f>
-        <v>Unit</v>
-      </c>
-      <c r="C3" s="16" t="str">
-        <f>CHAN!C3</f>
-        <v>Variable type</v>
-      </c>
-      <c r="D3" s="16" t="str">
-        <f>CHAN!D3</f>
-        <v>Note/comments</v>
-      </c>
-      <c r="E3" s="14" t="str">
-        <f>_xlfn.TEXTJOIN("_",,$A$1,E$1)</f>
-        <v>STR_MIX_1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="23">
-        <f>(0.00052534+0.00025201)*E7</f>
-        <v>7.5395176499999997E-4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E5" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E6" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="24">
-        <v>0.96989999999999998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" s="24">
-        <v>2.0846</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10" s="26" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="26">
-        <v>197.71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="E12" s="21" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="B13" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="E13" s="29">
-        <v>121508000000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="B14" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="E14" s="29">
-        <v>32.35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="E15" s="29">
-        <v>16.22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E16" s="22" t="b">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62FCDFC4-8F8B-44BE-BC94-0C08DE31F1F6}">
-  <dimension ref="A1:E12"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="18" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="67.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.81640625" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="14">
-        <f>SUM(E$2:Z2)</f>
-        <v>0</v>
-      </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" s="11">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1597,7 +1837,7 @@
       </c>
       <c r="E2" s="15">
         <f>IF(E$1 &gt; 0,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -1619,7 +1859,7 @@
       </c>
       <c r="E3" s="14" t="str">
         <f>_xlfn.TEXTJOIN("_",,$A$1,E$1)</f>
-        <v>STR_SC_0</v>
+        <v>STR_MIX_1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -1630,27 +1870,28 @@
         <v>6</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="13">
-        <v>0</v>
+        <v>33</v>
+      </c>
+      <c r="E4" s="23">
+        <f>(0.00052534+0.00025201)*E7</f>
+        <v>7.5395176499999997E-4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B5" s="22" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E5" s="23">
         <v>0</v>
@@ -1658,16 +1899,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B6" s="22" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E6" s="23">
         <v>0</v>
@@ -1678,107 +1919,175 @@
         <v>0</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="24">
+        <v>0.96989999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="24">
+        <v>2.0846</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="26">
+        <v>197.71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" s="29">
+        <v>121508000000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" s="29">
+        <v>32.35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="7">
-        <v>0.96989999999999998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="8" t="s">
+      <c r="C15" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B9" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="E9" s="29">
-        <v>170360000000000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="E10" s="21">
-        <v>30.23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="E11" s="21">
-        <v>16.73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E12" s="22" t="b">
-        <v>1</v>
+      <c r="E15" s="29">
+        <v>16.22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16" s="22" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1805,7 +2114,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B1" s="14">
         <f>SUM(E$2:Z2)</f>
@@ -1813,7 +2122,7 @@
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E1" s="2">
         <v>0</v>
@@ -1824,7 +2133,7 @@
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" s="14">
         <f>IF(E$1 &gt; 0,1,0)</f>
@@ -1861,10 +2170,10 @@
         <v>6</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E4" s="13">
         <v>0</v>
@@ -1872,16 +2181,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B5" s="22" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E5" s="23">
         <v>0</v>
@@ -1889,16 +2198,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B6" s="22" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E6" s="23">
         <v>0</v>
@@ -1909,13 +2218,13 @@
         <v>0</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E7" s="7">
         <v>0.96989999999999998</v>
@@ -1923,19 +2232,19 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -1943,13 +2252,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E9" s="12">
         <v>100</v>
@@ -1957,16 +2266,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E10" s="22" t="b">
         <v>1</v>
@@ -1983,7 +2292,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -2002,7 +2311,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="14">
         <f>SUM(E$2:Z2)</f>
@@ -2010,7 +2319,7 @@
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E1" s="11">
         <v>1</v>
@@ -2021,7 +2330,7 @@
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E2" s="15">
         <f>IF(E$1 &gt; 0,1,0)</f>
@@ -2052,16 +2361,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E4" s="6">
         <f>0.00030699</f>
@@ -2070,16 +2379,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E5" s="6">
         <v>2.7965999999999999E-4</v>
@@ -2087,16 +2396,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B6" s="22" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E6" s="23">
         <v>0</v>
@@ -2104,16 +2413,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B7" s="22" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E7" s="23">
         <v>0</v>
@@ -2121,16 +2430,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B8" s="22" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E8" s="23">
         <v>0</v>
@@ -2138,16 +2447,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B9" s="22" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E9" s="23">
         <v>0</v>
@@ -2155,16 +2464,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E10" s="12">
         <v>2</v>
@@ -2172,36 +2481,36 @@
     </row>
     <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="28" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -2209,10 +2518,10 @@
         <v>0</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E13" s="6">
         <v>1</v>
@@ -2220,33 +2529,33 @@
     </row>
     <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="28" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D14" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" s="27" t="s">
         <v>66</v>
-      </c>
-      <c r="E14" s="27" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E15" s="22">
         <v>1</v>
@@ -2254,16 +2563,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="E16" s="22" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
chore: new input parameters in sheet STR_MIX of file template_conductor_1_input
Added input parameters nn and E0 for the power law of the superconducting electrical resistivity.
</commit_message>
<xml_diff>
--- a/source_code/input_files/input_file_template/template_conductor_1_input.xlsx
+++ b/source_code/input_files/input_file_template/template_conductor_1_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/daniele_placido_polito_it/Documents/OPENSC2/source_code/input_files/input_file_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="280" documentId="13_ncr:1_{0BD40D79-8656-4BCB-943B-68FA050A86D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B79F21B8-56E2-4D4E-9ECB-A48BD02ED969}"/>
+  <xr:revisionPtr revIDLastSave="285" documentId="13_ncr:1_{0BD40D79-8656-4BCB-943B-68FA050A86D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{38B35361-7B9B-48B0-B3EB-0F9040D799AD}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CHAN" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="128">
   <si>
     <t>COSTETA</t>
   </si>
@@ -949,11 +949,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1349,11 +1349,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62FCDFC4-8F8B-44BE-BC94-0C08DE31F1F6}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomRight" activeCell="A24" sqref="A24:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1793,13 +1793,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomRight" activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2068,19 +2068,54 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="E16" s="21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="E17" s="21">
+        <f>10^-5</f>
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B16" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="22" t="s">
+      <c r="B18" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E16" s="22" t="b">
+      <c r="E18" s="22" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2099,7 +2134,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2296,7 +2331,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K24" sqref="K24"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
chore: update template input files
</commit_message>
<xml_diff>
--- a/source_code/input_files/input_file_template/template_conductor_1_input.xlsx
+++ b/source_code/input_files/input_file_template/template_conductor_1_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/daniele_placido_polito_it/Documents/OPENSC2/source_code/input_files/input_file_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="286" documentId="13_ncr:1_{0BD40D79-8656-4BCB-943B-68FA050A86D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{486F8D7B-5056-434C-81FC-AF9B6B2F8C67}"/>
+  <xr:revisionPtr revIDLastSave="291" documentId="13_ncr:1_{0BD40D79-8656-4BCB-943B-68FA050A86D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E169F1BB-0E35-40A5-97AD-BFC756F19BEB}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -222,12 +222,6 @@
     <t>Cu</t>
   </si>
   <si>
-    <t>steinless_steel</t>
-  </si>
-  <si>
-    <t>glass_epoxy</t>
-  </si>
-  <si>
     <t>Jacket_kind</t>
   </si>
   <si>
@@ -318,12 +312,6 @@
     <t>insulation_material</t>
   </si>
   <si>
-    <t>Flag, steinless_steel = steinless steel (old Fortran IJK); none = insulation component</t>
-  </si>
-  <si>
-    <t>Flag, glass_epoxy = glass epoxy; none = pure metal component</t>
-  </si>
-  <si>
     <t>flag for material: NbTi = niobiun titanium, Nb3Sn = niobium thin, YBCO = YBCO (REBCO)</t>
   </si>
   <si>
@@ -424,6 +412,18 @@
   </si>
   <si>
     <t>Number of materials constituting the tape.</t>
+  </si>
+  <si>
+    <t>ss</t>
+  </si>
+  <si>
+    <t>ge</t>
+  </si>
+  <si>
+    <t>Flag, ss = steinless steel (old Fortran IJK); none = insulation component</t>
+  </si>
+  <si>
+    <t>Flag, ge = glass epoxy; none = pure metal component</t>
   </si>
 </sst>
 </file>
@@ -1047,7 +1047,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B5" s="22" t="s">
         <v>7</v>
@@ -1056,7 +1056,7 @@
         <v>14</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E5" s="23">
         <v>0</v>
@@ -1067,7 +1067,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B6" s="22" t="s">
         <v>7</v>
@@ -1076,7 +1076,7 @@
         <v>14</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E6" s="23">
         <v>0</v>
@@ -1127,7 +1127,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B9" s="22" t="s">
         <v>7</v>
@@ -1136,7 +1136,7 @@
         <v>14</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E9" s="24">
         <v>0</v>
@@ -1320,7 +1320,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B19" s="22" t="s">
         <v>17</v>
@@ -1329,7 +1329,7 @@
         <v>54</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E19" s="22" t="b">
         <v>0</v>
@@ -1368,7 +1368,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B1" s="14">
         <f>SUM(E$2:Z2)</f>
@@ -1435,7 +1435,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="28" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B5" s="22" t="s">
         <v>7</v>
@@ -1444,7 +1444,7 @@
         <v>14</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E5" s="23">
         <v>0</v>
@@ -1452,7 +1452,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="28" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B6" s="22" t="s">
         <v>7</v>
@@ -1461,7 +1461,7 @@
         <v>14</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E6" s="23">
         <v>0</v>
@@ -1486,16 +1486,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="28" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B8" s="22" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D8" s="28" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E8" s="24">
         <v>1</v>
@@ -1503,7 +1503,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="28" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B9" s="22" t="s">
         <v>7</v>
@@ -1512,13 +1512,13 @@
         <v>14</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E9" s="24"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="28" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B10" s="22" t="s">
         <v>7</v>
@@ -1527,13 +1527,13 @@
         <v>14</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E10" s="24"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="28" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B11" s="22" t="s">
         <v>7</v>
@@ -1542,13 +1542,13 @@
         <v>14</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E11" s="24"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="28" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B12" s="22" t="s">
         <v>7</v>
@@ -1557,13 +1557,13 @@
         <v>14</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E12" s="24"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="28" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B13" s="22" t="s">
         <v>7</v>
@@ -1572,13 +1572,13 @@
         <v>14</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E13" s="24"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="28" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B14" s="22" t="s">
         <v>7</v>
@@ -1587,28 +1587,28 @@
         <v>14</v>
       </c>
       <c r="D14" s="28" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E14" s="24"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="28" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B15" s="22" t="s">
         <v>17</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D15" s="28" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E15" s="24"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="28" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B16" s="22" t="s">
         <v>17</v>
@@ -1617,13 +1617,13 @@
         <v>15</v>
       </c>
       <c r="D16" s="28" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E16" s="24"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="28" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B17" s="22" t="s">
         <v>17</v>
@@ -1632,13 +1632,13 @@
         <v>15</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E17" s="24"/>
     </row>
     <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="28" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B18" s="22" t="s">
         <v>17</v>
@@ -1647,13 +1647,13 @@
         <v>15</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E18" s="24"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="28" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B19" s="22" t="s">
         <v>17</v>
@@ -1662,13 +1662,13 @@
         <v>15</v>
       </c>
       <c r="D19" s="28" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E19" s="24"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="28" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B20" s="22" t="s">
         <v>17</v>
@@ -1677,13 +1677,13 @@
         <v>15</v>
       </c>
       <c r="D20" s="28" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E20" s="24"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="30" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B21" s="21" t="s">
         <v>21</v>
@@ -1692,7 +1692,7 @@
         <v>14</v>
       </c>
       <c r="D21" s="30" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E21" s="29">
         <v>170360000000000</v>
@@ -1700,7 +1700,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="30" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B22" s="21" t="s">
         <v>22</v>
@@ -1709,7 +1709,7 @@
         <v>14</v>
       </c>
       <c r="D22" s="30" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E22" s="21">
         <v>30.23</v>
@@ -1717,7 +1717,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="30" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B23" s="21" t="s">
         <v>18</v>
@@ -1726,7 +1726,7 @@
         <v>14</v>
       </c>
       <c r="D23" s="30" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E23" s="21">
         <v>16.73</v>
@@ -1734,16 +1734,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="D24" s="30" t="s">
         <v>116</v>
-      </c>
-      <c r="B24" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="D24" s="30" t="s">
-        <v>120</v>
       </c>
       <c r="E24" s="21">
         <v>20</v>
@@ -1751,16 +1751,16 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="30" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C25" s="21" t="s">
         <v>14</v>
       </c>
       <c r="D25" s="30" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E25" s="21">
         <f>10^-5</f>
@@ -1769,7 +1769,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="28" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B26" s="22" t="s">
         <v>17</v>
@@ -1778,7 +1778,7 @@
         <v>54</v>
       </c>
       <c r="D26" s="28" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E26" s="22" t="b">
         <v>1</v>
@@ -1882,7 +1882,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B5" s="22" t="s">
         <v>7</v>
@@ -1891,7 +1891,7 @@
         <v>14</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E5" s="23">
         <v>0</v>
@@ -1899,7 +1899,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B6" s="22" t="s">
         <v>7</v>
@@ -1908,7 +1908,7 @@
         <v>14</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E6" s="23">
         <v>0</v>
@@ -1967,7 +1967,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>17</v>
@@ -2001,7 +2001,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B12" s="21" t="s">
         <v>17</v>
@@ -2010,7 +2010,7 @@
         <v>15</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E12" s="21" t="s">
         <v>57</v>
@@ -2018,7 +2018,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B13" s="21" t="s">
         <v>21</v>
@@ -2027,7 +2027,7 @@
         <v>14</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E13" s="29">
         <v>121508000000</v>
@@ -2035,7 +2035,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B14" s="21" t="s">
         <v>22</v>
@@ -2044,7 +2044,7 @@
         <v>14</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E14" s="29">
         <v>32.35</v>
@@ -2052,7 +2052,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B15" s="21" t="s">
         <v>18</v>
@@ -2061,7 +2061,7 @@
         <v>14</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E15" s="29">
         <v>16.22</v>
@@ -2069,16 +2069,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" s="30" t="s">
         <v>116</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="D16" s="30" t="s">
-        <v>120</v>
       </c>
       <c r="E16" s="21">
         <v>20</v>
@@ -2086,16 +2086,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="30" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C17" s="21" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E17" s="21">
         <f>10^-5</f>
@@ -2104,7 +2104,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B18" s="22" t="s">
         <v>17</v>
@@ -2113,7 +2113,7 @@
         <v>54</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E18" s="22" t="b">
         <v>0</v>
@@ -2216,7 +2216,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B5" s="22" t="s">
         <v>7</v>
@@ -2225,7 +2225,7 @@
         <v>14</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E5" s="23">
         <v>0</v>
@@ -2233,7 +2233,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B6" s="22" t="s">
         <v>7</v>
@@ -2242,7 +2242,7 @@
         <v>14</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E6" s="23">
         <v>0</v>
@@ -2267,7 +2267,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>17</v>
@@ -2301,7 +2301,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B10" s="22" t="s">
         <v>17</v>
@@ -2310,7 +2310,7 @@
         <v>54</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E10" s="22" t="b">
         <v>1</v>
@@ -2331,7 +2331,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2396,7 +2396,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>6</v>
@@ -2414,7 +2414,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>6</v>
@@ -2431,7 +2431,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B6" s="22" t="s">
         <v>7</v>
@@ -2440,7 +2440,7 @@
         <v>14</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E6" s="23">
         <v>0</v>
@@ -2448,7 +2448,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B7" s="22" t="s">
         <v>7</v>
@@ -2457,7 +2457,7 @@
         <v>14</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E7" s="23">
         <v>0</v>
@@ -2465,7 +2465,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B8" s="22" t="s">
         <v>7</v>
@@ -2474,7 +2474,7 @@
         <v>14</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E8" s="23">
         <v>0</v>
@@ -2482,7 +2482,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B9" s="22" t="s">
         <v>7</v>
@@ -2491,7 +2491,7 @@
         <v>14</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E9" s="23">
         <v>0</v>
@@ -2516,7 +2516,7 @@
     </row>
     <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="28" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>17</v>
@@ -2525,15 +2525,15 @@
         <v>15</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>60</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>17</v>
@@ -2542,10 +2542,10 @@
         <v>15</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>93</v>
+        <v>127</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>61</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -2564,7 +2564,7 @@
     </row>
     <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="28" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B14" s="22" t="s">
         <v>17</v>
@@ -2573,15 +2573,15 @@
         <v>15</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E14" s="27" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B15" s="22" t="s">
         <v>17</v>
@@ -2590,7 +2590,7 @@
         <v>14</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E15" s="22">
         <v>1</v>
@@ -2598,7 +2598,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B16" s="22" t="s">
         <v>17</v>
@@ -2607,7 +2607,7 @@
         <v>54</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E16" s="22" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
chore: update sheet STR_MIX
Added the possibility to explicitly define mixed strand (stabilizer + supercondutor) and segregated stabilizer (as the number of strand and the corresponding diameter for a specific type).

Stabilizer non stabilizer ratio can be of two kinds:
    1. accounts for segregated stabilizer;
    2. does not account for segredated stabilizer
This is used to correctly evaluate the superconduciting cross section and
therefore the total stabilizer cross section used in the electric module.

The scaling parameter for the critical current density correlation c0 can be according to two different definitions (flag C0_MODE):
    1. ingegneristic, i.e., the value is normalized with respect to the total perpendicular cross section of superconducting strand (stabilizer + superconductor);
    2. physical, i.e., the value is normalized with respect to the total perpendicular cross section of supecronductor only
</commit_message>
<xml_diff>
--- a/source_code/input_files/input_file_template/template_conductor_1_input.xlsx
+++ b/source_code/input_files/input_file_template/template_conductor_1_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/daniele_placido_polito_it/Documents/OPENSC2/source_code/input_files/input_file_template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniele.placido\3D Objects\OPENSC2\source_code\input_files\input_file_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="291" documentId="13_ncr:1_{0BD40D79-8656-4BCB-943B-68FA050A86D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E169F1BB-0E35-40A5-97AD-BFC756F19BEB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B4B385-5418-4B43-AE1B-9EF3C9BF31E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11295" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CHAN" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="143">
   <si>
     <t>COSTETA</t>
   </si>
@@ -312,9 +312,6 @@
     <t>insulation_material</t>
   </si>
   <si>
-    <t>flag for material: NbTi = niobiun titanium, Nb3Sn = niobium thin, YBCO = YBCO (REBCO)</t>
-  </si>
-  <si>
     <t>STACK</t>
   </si>
   <si>
@@ -424,6 +421,54 @@
   </si>
   <si>
     <t>Flag, ge = glass epoxy; none = pure metal component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">perpendicular cross section </t>
+  </si>
+  <si>
+    <t>x coordinate of the barycenter</t>
+  </si>
+  <si>
+    <t>y coordinate of the barycenter</t>
+  </si>
+  <si>
+    <t>ISTAB_NON_STAB</t>
+  </si>
+  <si>
+    <t>flag to select the definition of the stabilizer not stabilizer ratio: 0 = definition does not accounts of segregated stabilizer strands; 1 = definition accounts of segregated stabilizer strands .</t>
+  </si>
+  <si>
+    <t>N_sc_strand</t>
+  </si>
+  <si>
+    <t>Number of superconducting strands</t>
+  </si>
+  <si>
+    <t>d_sc_strand</t>
+  </si>
+  <si>
+    <t>Diameter of superconducting strands</t>
+  </si>
+  <si>
+    <t>N_stab_strand</t>
+  </si>
+  <si>
+    <t>Number of stabilizer strands</t>
+  </si>
+  <si>
+    <t>d_stab_strand</t>
+  </si>
+  <si>
+    <t>Diameter of stabilizer strands</t>
+  </si>
+  <si>
+    <t>flag for material: NbTi = niobiun titanium, Nb3Sn = niobium thin, HTS = high critical temperature superconducting material, scaling.dat = scaling from file scaling.dat</t>
+  </si>
+  <si>
+    <t>C0_MODE</t>
+  </si>
+  <si>
+    <t>Flag for the definition scaling coefficient c0: 0 = engineering; 1 = physical; defaults to 0</t>
   </si>
 </sst>
 </file>
@@ -491,7 +536,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
@@ -519,14 +564,7 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -542,47 +580,15 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
@@ -591,18 +597,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -956,21 +950,21 @@
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="68" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="17.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.81640625" style="3"/>
+    <col min="5" max="6" width="17.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="14">
+      <c r="B1" s="12">
         <f>SUM(E$2:U$2)</f>
         <v>2</v>
       </c>
@@ -984,48 +978,48 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="D2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="12">
         <f>IF(E$1 &gt; 0,1,0)</f>
         <v>1</v>
       </c>
-      <c r="F2" s="14">
+      <c r="F2" s="12">
         <f>IF(F$1 &gt; 0,1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="16" t="str">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="str">
         <f>[1]TRANSIENT!A$2</f>
         <v>Variable name</v>
       </c>
-      <c r="B3" s="16" t="str">
+      <c r="B3" s="14" t="str">
         <f>[1]TRANSIENT!B$2</f>
         <v>Unit</v>
       </c>
-      <c r="C3" s="16" t="str">
+      <c r="C3" s="14" t="str">
         <f>[1]TRANSIENT!C$2</f>
         <v>Variable type</v>
       </c>
-      <c r="D3" s="16" t="str">
+      <c r="D3" s="14" t="str">
         <f>[1]TRANSIENT!D$2</f>
         <v>Note/comments</v>
       </c>
-      <c r="E3" s="14" t="str">
+      <c r="E3" s="12" t="str">
         <f>_xlfn.TEXTJOIN("_",,$A$1,E$1)</f>
         <v>CHAN_1</v>
       </c>
-      <c r="F3" s="14" t="str">
+      <c r="F3" s="12" t="str">
         <f>_xlfn.TEXTJOIN("_",,$A$1,F$1)</f>
         <v>CHAN_2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1035,57 +1029,57 @@
       <c r="C4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="6">
         <v>5.0265000000000001E-5</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="6">
         <v>3.6965000000000001E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E5" s="23">
-        <v>0</v>
-      </c>
-      <c r="F5" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E5" s="6">
+        <v>0</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E6" s="23">
-        <v>0</v>
-      </c>
-      <c r="F6" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E6" s="6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
@@ -1098,14 +1092,14 @@
       <c r="D7" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
@@ -1118,54 +1112,54 @@
       <c r="D8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="20">
+      <c r="E8" s="7">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="F8" s="20">
+      <c r="F8" s="7">
         <v>3.2676E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E9" s="24">
-        <v>0</v>
-      </c>
-      <c r="F9" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="9" t="s">
+      <c r="E9" s="7">
+        <v>0</v>
+      </c>
+      <c r="F9" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="5">
         <v>1</v>
       </c>
-      <c r="F10" s="21">
+      <c r="F10" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
@@ -1178,14 +1172,14 @@
       <c r="D11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E11" s="5">
         <v>1</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="5">
         <v>0.313</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
@@ -1198,15 +1192,15 @@
       <c r="D12" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="5">
         <v>-99</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F12" s="5">
         <v>-99</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="10" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -1218,14 +1212,14 @@
       <c r="D13" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E13" s="5">
         <v>0.02</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F13" s="5">
         <v>0.02</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>10</v>
       </c>
@@ -1235,16 +1229,16 @@
       <c r="C14" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E14" s="18" t="b">
+      <c r="E14" s="5" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="F14" s="18" t="b">
+      <c r="F14" s="5" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>11</v>
       </c>
@@ -1254,14 +1248,14 @@
       <c r="C15" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="19">
-        <v>0</v>
-      </c>
-      <c r="F15" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E15" s="6">
+        <v>0</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>12</v>
       </c>
@@ -1271,14 +1265,14 @@
       <c r="C16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="19">
-        <v>0</v>
-      </c>
-      <c r="F16" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E16" s="6">
+        <v>0</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>49</v>
       </c>
@@ -1298,7 +1292,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>55</v>
       </c>
@@ -1318,23 +1312,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B19" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="22" t="s">
+      <c r="B19" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>54</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="E19" s="22" t="b">
-        <v>0</v>
-      </c>
-      <c r="F19" s="22" t="b">
+      <c r="E19" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F19" s="5" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1356,21 +1350,21 @@
       <selection pane="bottomRight" activeCell="A24" sqref="A24:XFD25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="67.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.81640625" style="3"/>
+    <col min="2" max="2" width="7.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="67.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="B1" s="14">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="12">
         <f>SUM(E$2:Z2)</f>
         <v>0</v>
       </c>
@@ -1378,409 +1372,409 @@
       <c r="D1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="E1" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="13">
         <f>IF(E$1 &gt; 0,1,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="16" t="str">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="str">
         <f>CHAN!A3</f>
         <v>Variable name</v>
       </c>
-      <c r="B3" s="16" t="str">
+      <c r="B3" s="14" t="str">
         <f>CHAN!B3</f>
         <v>Unit</v>
       </c>
-      <c r="C3" s="16" t="str">
+      <c r="C3" s="14" t="str">
         <f>CHAN!C3</f>
         <v>Variable type</v>
       </c>
-      <c r="D3" s="16" t="str">
+      <c r="D3" s="14" t="str">
         <f>CHAN!D3</f>
         <v>Note/comments</v>
       </c>
-      <c r="E3" s="14" t="str">
+      <c r="E3" s="12" t="str">
         <f>_xlfn.TEXTJOIN("_",,$A$1,E$1)</f>
         <v>STACK_0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="28" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="28" t="s">
+      <c r="C4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="28" t="s">
+      <c r="E4" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="28" t="s">
+      <c r="C5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="E5" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="28" t="s">
+      <c r="E5" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="28" t="s">
+      <c r="C6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="E6" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="28" t="s">
+      <c r="E6" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="24">
+      <c r="E7" s="7">
         <v>0.96989999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="28" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B8" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="22" t="s">
+      <c r="D8" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="E8" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="E8" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="28" t="s">
+      <c r="B9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="E9" s="24"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="28" t="s">
+      <c r="C10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="28" t="s">
+      <c r="C11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="E10" s="24"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="28" t="s">
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B12" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="28" t="s">
+      <c r="C12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="E11" s="24"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="28" t="s">
+      <c r="E12" s="7"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B13" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="28" t="s">
+      <c r="C13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="E12" s="24"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="28" t="s">
+      <c r="E13" s="7"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B14" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="28" t="s">
+      <c r="C14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="E13" s="24"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="28" t="s">
+      <c r="E14" s="7"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="E15" s="7"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="B14" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="28" t="s">
-        <v>121</v>
-      </c>
-      <c r="E14" s="24"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="28" t="s">
-        <v>122</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="D15" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="E15" s="24"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="28" t="s">
+      <c r="B16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="E16" s="7"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="B16" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="22" t="s">
+      <c r="B17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="28" t="s">
+      <c r="D17" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="E16" s="24"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="28" t="s">
+      <c r="E17" s="7"/>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="B17" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="22" t="s">
+      <c r="B18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="28" t="s">
+      <c r="D18" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="E18" s="7"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="E17" s="24"/>
-    </row>
-    <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="28" t="s">
-        <v>104</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="22" t="s">
+      <c r="E19" s="7"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="E18" s="24"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="B19" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" s="28" t="s">
+      <c r="D20" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="E19" s="24"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="B20" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="28" t="s">
+      <c r="E20" s="7"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" s="6">
+        <v>170360000000000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" s="5">
+        <v>30.23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23" s="5">
+        <v>16.73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="E20" s="24"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="B21" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="E21" s="29">
-        <v>170360000000000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="B22" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="E22" s="21">
-        <v>30.23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="B23" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="E23" s="21">
-        <v>16.73</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="30" t="s">
+      <c r="B24" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="E24" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="B24" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="D24" s="30" t="s">
-        <v>116</v>
-      </c>
-      <c r="E24" s="21">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="30" t="s">
+      <c r="B25" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B25" s="21" t="s">
+      <c r="C25" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="C25" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" s="30" t="s">
-        <v>115</v>
-      </c>
-      <c r="E25" s="21">
+      <c r="E25" s="5">
         <f>10^-5</f>
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="28" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B26" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C26" s="22" t="s">
+      <c r="B26" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D26" s="28" t="s">
+      <c r="D26" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="E26" s="22" t="b">
+      <c r="E26" s="5" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1793,30 +1787,30 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="67.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="67.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.81640625" style="3"/>
+    <col min="6" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="14">
+      <c r="B1" s="12">
         <f>SUM(E$2:U2)</f>
         <v>1</v>
       </c>
@@ -1824,45 +1818,45 @@
       <c r="D1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="11">
+      <c r="E1" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="13">
         <f>IF(E$1 &gt; 0,1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="16" t="str">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="str">
         <f>CHAN!A3</f>
         <v>Variable name</v>
       </c>
-      <c r="B3" s="16" t="str">
+      <c r="B3" s="14" t="str">
         <f>CHAN!B3</f>
         <v>Unit</v>
       </c>
-      <c r="C3" s="16" t="str">
+      <c r="C3" s="14" t="str">
         <f>CHAN!C3</f>
         <v>Variable type</v>
       </c>
-      <c r="D3" s="16" t="str">
+      <c r="D3" s="14" t="str">
         <f>CHAN!D3</f>
         <v>Note/comments</v>
       </c>
-      <c r="E3" s="14" t="str">
+      <c r="E3" s="12" t="str">
         <f>_xlfn.TEXTJOIN("_",,$A$1,E$1)</f>
         <v>STR_MIX_1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1873,48 +1867,48 @@
         <v>14</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="23">
+        <v>127</v>
+      </c>
+      <c r="E4" s="6">
         <f>(0.00052534+0.00025201)*E7</f>
         <v>7.5395176499999997E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E5" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+        <v>128</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E6" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+        <v>129</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
@@ -1927,196 +1921,280 @@
       <c r="D7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="24">
+      <c r="E7" s="7">
         <v>0.96989999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E8" s="7">
+        <v>2.0846</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="B9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="24">
-        <v>2.0846</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
+      <c r="E9" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="5" t="s">
+      <c r="B10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+      <c r="E10" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E11" s="16">
+        <v>197.71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E13" s="6">
+        <v>121508000000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E14" s="6">
+        <v>32.35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="22" t="s">
+      <c r="B15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E10" s="26" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
+      <c r="E15" s="6">
+        <v>16.22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="3" t="s">
+      <c r="B16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="26">
-        <v>197.71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="8" t="s">
+      <c r="E16" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B12" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="21" t="s">
+      <c r="B17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="E12" s="21" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="B13" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E13" s="29">
-        <v>121508000000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B14" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E14" s="29">
-        <v>32.35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E15" s="29">
-        <v>16.22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="30" t="s">
-        <v>112</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="D16" s="30" t="s">
-        <v>116</v>
-      </c>
-      <c r="E16" s="21">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="30" t="s">
-        <v>113</v>
-      </c>
-      <c r="B17" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="30" t="s">
-        <v>115</v>
-      </c>
-      <c r="E17" s="21">
+      <c r="D17" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="E17" s="5">
         <f>10^-5</f>
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E18" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B18" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="22" t="s">
+      <c r="B24" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D24" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="E18" s="22" t="b">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2137,21 +2215,21 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.81640625" style="3"/>
+    <col min="1" max="1" width="13.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="14">
+      <c r="B1" s="12">
         <f>SUM(E$2:Z2)</f>
         <v>0</v>
       </c>
@@ -2163,41 +2241,41 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="12">
         <f>IF(E$1 &gt; 0,1,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="16" t="str">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="str">
         <f>CHAN!A3</f>
         <v>Variable name</v>
       </c>
-      <c r="B3" s="16" t="str">
+      <c r="B3" s="14" t="str">
         <f>CHAN!B3</f>
         <v>Unit</v>
       </c>
-      <c r="C3" s="16" t="str">
+      <c r="C3" s="14" t="str">
         <f>CHAN!C3</f>
         <v>Variable type</v>
       </c>
-      <c r="D3" s="16" t="str">
+      <c r="D3" s="14" t="str">
         <f>CHAN!D3</f>
         <v>Note/comments</v>
       </c>
-      <c r="E3" s="14" t="str">
+      <c r="E3" s="12" t="str">
         <f>_xlfn.TEXTJOIN("_",,$A$1,E$1)</f>
         <v>STR_STAB_0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -2210,45 +2288,45 @@
       <c r="D4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E4" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E5" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E5" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E6" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E6" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
@@ -2265,24 +2343,24 @@
         <v>0.96989999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>84</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="E8" s="16" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
@@ -2295,24 +2373,24 @@
       <c r="D9" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="10">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B10" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="22" t="s">
+      <c r="B10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>54</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E10" s="22" t="b">
+      <c r="E10" s="5" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2331,24 +2409,24 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomRight" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.81640625" style="3"/>
+    <col min="1" max="1" width="20.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="14">
+      <c r="B1" s="12">
         <f>SUM(E$2:Z2)</f>
         <v>1</v>
       </c>
@@ -2356,45 +2434,45 @@
       <c r="D1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="11">
+      <c r="E1" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="13">
         <f>IF(E$1 &gt; 0,1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="16" t="str">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="str">
         <f>CHAN!A3</f>
         <v>Variable name</v>
       </c>
-      <c r="B3" s="16" t="str">
+      <c r="B3" s="14" t="str">
         <f>CHAN!B3</f>
         <v>Unit</v>
       </c>
-      <c r="C3" s="16" t="str">
+      <c r="C3" s="14" t="str">
         <f>CHAN!C3</f>
         <v>Variable type</v>
       </c>
-      <c r="D3" s="16" t="str">
+      <c r="D3" s="14" t="str">
         <f>CHAN!D3</f>
         <v>Note/comments</v>
       </c>
-      <c r="E3" s="14" t="str">
+      <c r="E3" s="12" t="str">
         <f>_xlfn.TEXTJOIN("_",,$A$1,E$1)</f>
         <v>Z_JACKET_1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>86</v>
       </c>
@@ -2412,7 +2490,7 @@
         <v>3.0698999999999999E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>87</v>
       </c>
@@ -2429,75 +2507,75 @@
         <v>2.7965999999999999E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E6" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E6" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E7" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E7" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E8" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E9" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E9" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>30</v>
       </c>
@@ -2510,12 +2588,12 @@
       <c r="D10" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="28" t="s">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
         <v>88</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -2525,13 +2603,13 @@
         <v>15</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+        <v>125</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>89</v>
       </c>
@@ -2542,13 +2620,13 @@
         <v>15</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>0</v>
       </c>
@@ -2562,54 +2640,54 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="28" t="s">
+    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B14" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="22" t="s">
+      <c r="B14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="27" t="s">
+      <c r="E14" s="17" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="22" t="s">
+      <c r="B15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E15" s="22">
+      <c r="E15" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B16" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="22" t="s">
+      <c r="B16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>54</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E16" s="22" t="b">
+      <c r="E16" s="5" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>